<commit_message>
2nd commit of doc for the project
</commit_message>
<xml_diff>
--- a/P05/Scrum_MICE.xlsx
+++ b/P05/Scrum_MICE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Desktop\Shared Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED8AC35-43AC-4448-9B3C-7B599056468A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876A2B5F-92C3-4873-B63A-6FFC1C07AB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="191">
   <si>
     <t>Product Name:</t>
   </si>
@@ -588,6 +588,33 @@
   </si>
   <si>
     <t>In Test</t>
+  </si>
+  <si>
+    <t>Made new Ice cream flavor</t>
+  </si>
+  <si>
+    <t>Made new Mixin Flavor</t>
+  </si>
+  <si>
+    <t>Made Mixin request</t>
+  </si>
+  <si>
+    <t>Made scoop of ice cream</t>
+  </si>
+  <si>
+    <t>Used menu to create new items (mixins/flavors/scoops)</t>
+  </si>
+  <si>
+    <t>In Work</t>
+  </si>
+  <si>
+    <t>Completed Day 6</t>
+  </si>
+  <si>
+    <t>Completed Day 7</t>
+  </si>
+  <si>
+    <t>Create multiple servings of scoops</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1288,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -1338,28 +1365,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1409,7 +1436,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -1483,7 +1510,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -1574,7 +1601,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -1722,7 +1749,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -1796,7 +1823,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -3709,7 +3736,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -5702,8 +5729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -5804,8 +5831,7 @@
         <v>164</v>
       </c>
       <c r="B7" s="18">
-        <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -5820,7 +5846,7 @@
       </c>
       <c r="B8" s="18">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C8" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5838,7 +5864,7 @@
       </c>
       <c r="B9" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C9" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5856,7 +5882,7 @@
       </c>
       <c r="B10" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C10" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5874,7 +5900,7 @@
       </c>
       <c r="B11" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C11" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5892,7 +5918,7 @@
       </c>
       <c r="B12" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C12" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5909,12 +5935,11 @@
         <v>170</v>
       </c>
       <c r="B13" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
@@ -5927,12 +5952,11 @@
         <v>171</v>
       </c>
       <c r="B14" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
@@ -5974,51 +5998,103 @@
       <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>180</v>
+      </c>
       <c r="D17" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="E17" s="28"/>
+        <v>182</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
         <v>3</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="28"/>
+      <c r="B19" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
         <v>4</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="28"/>
+      <c r="B20" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
         <v>5</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="28"/>
+      <c r="B21" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
         <v>6</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="28"/>
+      <c r="B22" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">

</xml_diff>